<commit_message>
update uts terakhir pos
</commit_message>
<xml_diff>
--- a/PWL_POS/public/template_penjualan.xlsx
+++ b/PWL_POS/public/template_penjualan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\Pemrograman_Web_Lanjut_2B_06\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7132C76-FD62-4C8B-A568-CE76AE8361DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC32EEA-6BB0-414B-9822-DAF16DB6B535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4344" yWindow="2496" windowWidth="17280" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3996" yWindow="2148" windowWidth="17280" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master Penjualan" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,6 @@
     <t>Tanggal Penjualan</t>
   </si>
   <si>
-    <t>Adib</t>
-  </si>
-  <si>
     <t>2025-04-21 13:13:52</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>PJN0015</t>
+  </si>
+  <si>
+    <t>Cahya</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,7 +441,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -458,13 +458,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -472,13 +472,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -486,13 +486,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -500,13 +500,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -514,13 +514,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -550,18 +550,18 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -589,7 +589,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -617,7 +617,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -659,7 +659,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -687,7 +687,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>5</v>

</xml_diff>